<commit_message>
primers git commit -m primers
</commit_message>
<xml_diff>
--- a/primers/sybr_primers.xlsx
+++ b/primers/sybr_primers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="600" windowWidth="28540" windowHeight="9160" tabRatio="500"/>
+    <workbookView xWindow="6640" yWindow="600" windowWidth="21860" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="140">
   <si>
     <t>Neuronal calcium sensor 1, Ncs1</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>ribosomal protein L19, rpl19</t>
-  </si>
-  <si>
-    <t>18S ribosomal RNA, Rn18S</t>
   </si>
   <si>
     <t>fragile X mental retardation syndrome 1, fmr1</t>
@@ -767,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,271 +781,294 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>61.2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>61.2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>62.8</v>
       </c>
       <c r="H3">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G4">
-        <v>62.8</v>
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D5">
-        <v>60</v>
+        <v>61.8</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G5">
-        <v>60</v>
-      </c>
-      <c r="H5">
-        <v>88</v>
+        <v>61.5</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>296</v>
+      </c>
+      <c r="I6" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6">
-        <v>61.8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>61.5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>60</v>
       </c>
-      <c r="E7" t="s">
-        <v>58</v>
+      <c r="E7" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G7">
         <v>60</v>
       </c>
       <c r="H7">
-        <v>296</v>
+        <v>171</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>60</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>66</v>
+      <c r="E8" t="s">
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H8">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
-        <v>68</v>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G9">
-        <v>62</v>
-      </c>
-      <c r="H9">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="H10">
+        <v>143</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11">
         <v>62</v>
@@ -1057,42 +1077,42 @@
         <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G11">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D12">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G12">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H12">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="I12" t="s">
         <v>88</v>
@@ -1100,380 +1120,355 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D13">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G13">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H13">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I13" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D14">
         <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G14">
         <v>60</v>
       </c>
       <c r="H14">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D15">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G15">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H15">
-        <v>101</v>
+        <v>173</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D16">
         <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G16">
         <v>61</v>
       </c>
-      <c r="H16">
-        <v>173</v>
-      </c>
       <c r="I16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D17">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G17">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
       </c>
       <c r="I17" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D18">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G18">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="D19">
-        <v>60</v>
+        <v>60.1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="G19">
-        <v>60</v>
+        <v>62.1</v>
       </c>
       <c r="H19">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I19" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="D20">
-        <v>60.1</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="G20">
-        <v>62.1</v>
+        <v>61</v>
       </c>
       <c r="H20">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="I20" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D21">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G21">
         <v>61</v>
       </c>
       <c r="H21">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D22">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22">
+        <v>62</v>
+      </c>
+      <c r="H22">
+        <v>107</v>
+      </c>
+      <c r="I22" t="s">
         <v>128</v>
-      </c>
-      <c r="F22" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22">
-        <v>61</v>
-      </c>
-      <c r="H22">
-        <v>191</v>
-      </c>
-      <c r="I22" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D23">
         <v>60</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G23">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H23">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I23" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
         <v>136</v>
       </c>
-      <c r="C24" t="s">
-        <v>133</v>
-      </c>
       <c r="D24">
         <v>60</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G24">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H24">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25">
-        <v>60</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" t="s">
-        <v>138</v>
-      </c>
-      <c r="G25">
-        <v>61</v>
-      </c>
-      <c r="H25">
-        <v>204</v>
-      </c>
-      <c r="I25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+      <c r="A25" s="1"/>
+    </row>
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
@@ -1486,10 +1481,6 @@
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G40">

</xml_diff>